<commit_message>
13-Apr-2024: configuration file and draw_ques.py were modified to handle boundary cases.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/PycharmProjects/MC_Test_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79D5BADE-B5A2-9749-907B-DFB2D7620088}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965F8BF5-B694-434D-BFE7-E200552F2038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="2960" windowWidth="27640" windowHeight="16940" xr2:uid="{23C2DCD3-4BA3-BF4E-8E61-67131C598746}"/>
+    <workbookView xWindow="10760" yWindow="880" windowWidth="27640" windowHeight="16940" xr2:uid="{23C2DCD3-4BA3-BF4E-8E61-67131C598746}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>questions.xlsx</t>
   </si>
@@ -62,28 +62,34 @@
     <t>last group</t>
   </si>
   <si>
+    <t>first category</t>
+  </si>
+  <si>
+    <t>A</t>
+  </si>
+  <si>
+    <t>questions per category</t>
+  </si>
+  <si>
+    <t>question bank</t>
+  </si>
+  <si>
+    <t>last category</t>
+  </si>
+  <si>
+    <t>mid group</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>P</t>
   </si>
   <si>
-    <t>first category</t>
-  </si>
-  <si>
-    <t>A</t>
-  </si>
-  <si>
     <t>H</t>
   </si>
   <si>
-    <t>questions per category</t>
-  </si>
-  <si>
     <t>10, 10, 10, 10, 15, 15, 15, 15</t>
-  </si>
-  <si>
-    <t>question bank</t>
-  </si>
-  <si>
-    <t>last category</t>
   </si>
 </sst>
 </file>
@@ -125,9 +131,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -462,10 +471,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D002EF5-4EA2-7847-B581-A7A8C1384107}">
-  <dimension ref="A1:B8"/>
+  <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -476,7 +485,7 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -492,26 +501,26 @@
     </row>
     <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>8</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>10</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>15</v>
+        <v>8</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
@@ -519,22 +528,30 @@
         <v>12</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>3</v>
+        <v>10</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>2</v>
       </c>
     </row>

</xml_diff>

<commit_message>
15-Apr-2024: Language is now specified in config.xlsx so that different fonts are used to generate the pdf file.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/PycharmProjects/MC_Test_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{965F8BF5-B694-434D-BFE7-E200552F2038}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F75A78-88C8-D34B-A626-DC04DA3AB828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="880" windowWidth="27640" windowHeight="16940" xr2:uid="{23C2DCD3-4BA3-BF4E-8E61-67131C598746}"/>
+    <workbookView xWindow="10760" yWindow="2960" windowWidth="27640" windowHeight="16940" xr2:uid="{23C2DCD3-4BA3-BF4E-8E61-67131C598746}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,10 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
-  <si>
-    <t>questions.xlsx</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>marksheet</t>
   </si>
@@ -90,6 +87,27 @@
   </si>
   <si>
     <t>10, 10, 10, 10, 15, 15, 15, 15</t>
+  </si>
+  <si>
+    <t>candidates.xlsx</t>
+  </si>
+  <si>
+    <t>scores.xlsx</t>
+  </si>
+  <si>
+    <t>test results</t>
+  </si>
+  <si>
+    <t>candidates data</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>example_ques.xlsx</t>
+  </si>
+  <si>
+    <t>English</t>
   </si>
 </sst>
 </file>
@@ -471,10 +489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D002EF5-4EA2-7847-B581-A7A8C1384107}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,74 +503,98 @@
   <sheetData>
     <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>13</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>8</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>3</v>
+        <v>20</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>1</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
16-Apr-2024: GUI implemented to load the configuration file and specify how many test paper to be generated.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/PycharmProjects/MC_Test_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91F75A78-88C8-D34B-A626-DC04DA3AB828}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DBC90D-9440-3B4A-A908-ECCF12BDCC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10760" yWindow="2960" windowWidth="27640" windowHeight="16940" xr2:uid="{23C2DCD3-4BA3-BF4E-8E61-67131C598746}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{23C2DCD3-4BA3-BF4E-8E61-67131C598746}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,17 +36,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>marksheet</t>
   </si>
   <si>
-    <t>marksheet.xlsx</t>
-  </si>
-  <si>
-    <t>testpaper.pdf</t>
-  </si>
-  <si>
     <t>M</t>
   </si>
   <si>
@@ -68,46 +62,61 @@
     <t>questions per category</t>
   </si>
   <si>
+    <t>last category</t>
+  </si>
+  <si>
+    <t>mid group</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
+    <t>P</t>
+  </si>
+  <si>
+    <t>H</t>
+  </si>
+  <si>
+    <t>10, 10, 10, 10, 15, 15, 15, 15</t>
+  </si>
+  <si>
+    <t>candidates.xlsx</t>
+  </si>
+  <si>
+    <t>scores.xlsx</t>
+  </si>
+  <si>
+    <t>test results</t>
+  </si>
+  <si>
+    <t>candidates data</t>
+  </si>
+  <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>example_ques.xlsx</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>; online test</t>
+  </si>
+  <si>
+    <t>; paper test</t>
+  </si>
+  <si>
+    <t>testpaper</t>
+  </si>
+  <si>
+    <t>the file type (pdf) will be added by the program</t>
+  </si>
+  <si>
+    <t>the file type (xlsx) will be added by the program</t>
+  </si>
+  <si>
     <t>question bank</t>
-  </si>
-  <si>
-    <t>last category</t>
-  </si>
-  <si>
-    <t>mid group</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>H</t>
-  </si>
-  <si>
-    <t>10, 10, 10, 10, 15, 15, 15, 15</t>
-  </si>
-  <si>
-    <t>candidates.xlsx</t>
-  </si>
-  <si>
-    <t>scores.xlsx</t>
-  </si>
-  <si>
-    <t>test results</t>
-  </si>
-  <si>
-    <t>candidates data</t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>example_ques.xlsx</t>
-  </si>
-  <si>
-    <t>English</t>
   </si>
 </sst>
 </file>
@@ -489,11 +498,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D002EF5-4EA2-7847-B581-A7A8C1384107}">
-  <dimension ref="A1:B12"/>
+  <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -501,100 +508,121 @@
     <col min="2" max="2" width="28.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B1" s="1" t="s">
+    </row>
+    <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A2" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B2" s="1" t="s">
+    <row r="11" spans="1:4" ht="19" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="B11" s="1" t="s">
         <v>23</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>5</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" ht="19" x14ac:dyDescent="0.25">
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>1</v>
+        <v>0</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
17-Apr-2024: Add Exit button in tkinter window.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/PycharmProjects/MC_Test_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{45DBC90D-9440-3B4A-A908-ECCF12BDCC45}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94FD92A-4DC3-2747-BCB5-BC90653A434C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{23C2DCD3-4BA3-BF4E-8E61-67131C598746}"/>
   </bookViews>
@@ -77,9 +77,6 @@
     <t>H</t>
   </si>
   <si>
-    <t>10, 10, 10, 10, 15, 15, 15, 15</t>
-  </si>
-  <si>
     <t>candidates.xlsx</t>
   </si>
   <si>
@@ -117,6 +114,9 @@
   </si>
   <si>
     <t>question bank</t>
+  </si>
+  <si>
+    <t>5, 5, 5, 5, 3, 3, 3</t>
   </si>
 </sst>
 </file>
@@ -500,7 +500,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D002EF5-4EA2-7847-B581-A7A8C1384107}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B7" sqref="B7"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -510,10 +512,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -561,40 +563,40 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>13</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C9" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -602,13 +604,13 @@
         <v>3</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
         <v>23</v>
-      </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
-      <c r="D11" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -619,10 +621,10 @@
         <v>0</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D12" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
24-Apr-2024: Minor change in draw_ques.py to take care of invalid entry in config.sys.
</commit_message>
<xml_diff>
--- a/config.xlsx
+++ b/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/steve/PycharmProjects/MC_Test_paper/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94FD92A-4DC3-2747-BCB5-BC90653A434C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8ADCB7-FF67-1F44-892F-EB722CD47023}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="38400" windowHeight="19400" xr2:uid="{23C2DCD3-4BA3-BF4E-8E61-67131C598746}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="38400" windowHeight="19400" xr2:uid="{23C2DCD3-4BA3-BF4E-8E61-67131C598746}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
   <si>
     <t>marksheet</t>
   </si>
@@ -68,6 +68,33 @@
     <t>mid group</t>
   </si>
   <si>
+    <t>language</t>
+  </si>
+  <si>
+    <t>example_ques.xlsx</t>
+  </si>
+  <si>
+    <t>English</t>
+  </si>
+  <si>
+    <t>; paper test</t>
+  </si>
+  <si>
+    <t>testpaper</t>
+  </si>
+  <si>
+    <t>the file type (pdf) will be added by the program</t>
+  </si>
+  <si>
+    <t>the file type (xlsx) will be added by the program</t>
+  </si>
+  <si>
+    <t>question bank</t>
+  </si>
+  <si>
+    <t>5, 5, 5, 5, 3, 3, 3</t>
+  </si>
+  <si>
     <t>N</t>
   </si>
   <si>
@@ -75,48 +102,6 @@
   </si>
   <si>
     <t>H</t>
-  </si>
-  <si>
-    <t>candidates.xlsx</t>
-  </si>
-  <si>
-    <t>scores.xlsx</t>
-  </si>
-  <si>
-    <t>test results</t>
-  </si>
-  <si>
-    <t>candidates data</t>
-  </si>
-  <si>
-    <t>language</t>
-  </si>
-  <si>
-    <t>example_ques.xlsx</t>
-  </si>
-  <si>
-    <t>English</t>
-  </si>
-  <si>
-    <t>; online test</t>
-  </si>
-  <si>
-    <t>; paper test</t>
-  </si>
-  <si>
-    <t>testpaper</t>
-  </si>
-  <si>
-    <t>the file type (pdf) will be added by the program</t>
-  </si>
-  <si>
-    <t>the file type (xlsx) will be added by the program</t>
-  </si>
-  <si>
-    <t>question bank</t>
-  </si>
-  <si>
-    <t>5, 5, 5, 5, 3, 3, 3</t>
   </si>
 </sst>
 </file>
@@ -498,10 +483,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D002EF5-4EA2-7847-B581-A7A8C1384107}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -512,10 +497,10 @@
   <sheetData>
     <row r="1" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -531,7 +516,7 @@
         <v>9</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -539,7 +524,7 @@
         <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -555,7 +540,7 @@
         <v>8</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>12</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="19" x14ac:dyDescent="0.25">
@@ -563,68 +548,46 @@
         <v>7</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>18</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="B8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C8" t="s">
         <v>13</v>
-      </c>
-      <c r="C8" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" t="s">
+        <v>13</v>
+      </c>
+      <c r="D9" t="s">
         <v>15</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="C9" t="s">
-        <v>20</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="19" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>19</v>
+        <v>0</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
       </c>
       <c r="C10" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C11" t="s">
-        <v>21</v>
-      </c>
-      <c r="D11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="19" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="C12" t="s">
-        <v>21</v>
-      </c>
-      <c r="D12" t="s">
-        <v>24</v>
+        <v>13</v>
+      </c>
+      <c r="D10" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>